<commit_message>
Orte/Places import + Matching for Ausstellungen
</commit_message>
<xml_diff>
--- a/Excel_Mapping/Mapping/Import_Mapping_ausstellung.xlsx
+++ b/Excel_Mapping/Mapping/Import_Mapping_ausstellung.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="115">
   <si>
     <t xml:space="preserve">Rule type</t>
   </si>
@@ -79,9 +79,29 @@
     <t xml:space="preserve">ca_occurrences.date</t>
   </si>
   <si>
+    <t xml:space="preserve">{"skipIfExpression":"^3 !~ /dddd/"} </t>
+  </si>
+  <si>
     <t xml:space="preserve">ca_occurrences.internal_notes</t>
   </si>
   <si>
+    <t xml:space="preserve">ca_places</t>
+  </si>
+  <si>
+    <t xml:space="preserve">placeSplitter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+ "delimiter": ";",
+ "placeType": "city",
+ "placeHierarchy": "root",
+ "relationshipType": "location",
+ "matchOn": ["labels"],
+ "ignoreParent": "1",
+ "dontCreate": "1"
+} </t>
+  </si>
+  <si>
     <t xml:space="preserve">Setting name</t>
   </si>
   <si>
@@ -272,9 +292,6 @@
   </si>
   <si>
     <t xml:space="preserve">CollectiveAccess</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ca_places</t>
   </si>
   <si>
     <t xml:space="preserve">merge_on_preferred_labels_with_replace</t>
@@ -377,7 +394,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -402,81 +419,21 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -497,57 +454,15 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF222222"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -555,23 +470,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -595,61 +495,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -669,7 +521,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -677,7 +533,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -685,7 +545,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -693,49 +553,29 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="22">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -747,7 +587,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -763,7 +603,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -775,11 +615,11 @@
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF222222"/>
+      <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF222222"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -792,8 +632,8 @@
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -807,7 +647,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="27.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="18.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="23.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="39.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="39.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="67.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="10.83"/>
   </cols>
@@ -870,7 +710,7 @@
       </c>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -880,242 +720,259 @@
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" s="6" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="G5" s="8"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="3"/>
+    <row r="6" customFormat="false" ht="87.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
-      <c r="G7" s="8"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="G8" s="8"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="8"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="8"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="8"/>
+      <c r="G12" s="10"/>
     </row>
     <row r="13" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" s="3" customFormat="true" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="10"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="11"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="11"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0</v>
@@ -1168,7 +1025,7 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -1182,235 +1039,235 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>61</v>
+      <c r="A2" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>19</v>
+      <c r="A3" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>67</v>
+      <c r="A4" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>71</v>
+      <c r="A5" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>74</v>
+      <c r="A6" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E16" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E17" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E19" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>